<commit_message>
Added Icons and improved design changes
</commit_message>
<xml_diff>
--- a/translations/Translations.xlsx
+++ b/translations/Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabri\Documents\GodotProject\GoDot game sw\translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ABB2D20-9C9E-44E6-9483-9C2A2380716E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22D11F18-BEB2-47ED-8077-818E2020885E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{113493BD-09A1-4BC8-836C-5C0414668FD8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="211">
   <si>
     <t>key</t>
   </si>
@@ -446,41 +446,6 @@
     <t>再開する</t>
   </si>
   <si>
-    <t>Designed and programmed
-by
-Fabrice Bäder</t>
-  </si>
-  <si>
-    <t>Entworfen und programmiert
-von
-Fabrice Bäder</t>
-  </si>
-  <si>
-    <t>Conçu et programmé
-par
-Fabrice bäder</t>
-  </si>
-  <si>
-    <t>Diseñado y programado
-por
-Fabrice Bäder</t>
-  </si>
-  <si>
-    <t>Ontworpen en geprogrammeerd
-door
-Fabrice Bäder</t>
-  </si>
-  <si>
-    <t>Progettato e programmato
-da
-Fabrice Bäder</t>
-  </si>
-  <si>
-    <t>Fabrice Bäder
-による
-デザインとプログラム</t>
-  </si>
-  <si>
     <t>Opnieuw opstarten</t>
   </si>
   <si>
@@ -586,11 +551,6 @@
     <t>Språk:</t>
   </si>
   <si>
-    <t>Designad och programmerad_x000D_
-av_x000D_
-Fabrice Bäder</t>
-  </si>
-  <si>
     <t>Fortsätt spelet</t>
   </si>
   <si>
@@ -682,6 +642,33 @@
   </si>
   <si>
     <t>Difficoltà (prossima partita):</t>
+  </si>
+  <si>
+    <t>Designed and programmed\nby\nFabrice Bäder</t>
+  </si>
+  <si>
+    <t>credits_text</t>
+  </si>
+  <si>
+    <t>Entworfen und programmiert\nvon\nFabrice Bäder</t>
+  </si>
+  <si>
+    <t>Conçu et programmé\npar\nFabrice bäder</t>
+  </si>
+  <si>
+    <t>Diseñado y programado\npor\nFabrice Bäder</t>
+  </si>
+  <si>
+    <t>Ontworpen en geprogrammeerd\ndoor\nFabrice Bäder</t>
+  </si>
+  <si>
+    <t>Progettato e programmato\nda\nFabrice Bäder</t>
+  </si>
+  <si>
+    <t>Designad och programmerad\nav\nFabrice Bäder</t>
+  </si>
+  <si>
+    <t>Fabrice Bäder\nによる\nデザインとプログラム</t>
   </si>
 </sst>
 </file>
@@ -1058,8 +1045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02BF2502-15EB-43B9-AACE-3B572B58F446}">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="F2" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1101,7 +1088,7 @@
         <v>9</v>
       </c>
       <c r="I1" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -1130,7 +1117,7 @@
         <v>11</v>
       </c>
       <c r="I2" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -1159,7 +1146,7 @@
         <v>18</v>
       </c>
       <c r="I3" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -1188,7 +1175,7 @@
         <v>25</v>
       </c>
       <c r="I4" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -1199,25 +1186,25 @@
         <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="D5" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="E5" t="s">
         <v>27</v>
       </c>
       <c r="F5" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="G5" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="H5" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="I5" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -1225,28 +1212,28 @@
         <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="C6" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="D6" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="E6" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="F6" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="G6" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="H6" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="I6" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -1275,7 +1262,7 @@
         <v>76</v>
       </c>
       <c r="I7" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -1362,7 +1349,7 @@
         <v>79</v>
       </c>
       <c r="I10" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -1391,7 +1378,7 @@
         <v>80</v>
       </c>
       <c r="I11" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -1420,7 +1407,7 @@
         <v>81</v>
       </c>
       <c r="I12" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -1449,7 +1436,7 @@
         <v>82</v>
       </c>
       <c r="I13" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -1478,7 +1465,7 @@
         <v>83</v>
       </c>
       <c r="I14" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -1507,7 +1494,7 @@
         <v>84</v>
       </c>
       <c r="I15" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -1536,7 +1523,7 @@
         <v>85</v>
       </c>
       <c r="I16" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
@@ -1565,36 +1552,36 @@
         <v>86</v>
       </c>
       <c r="I17" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="B18" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="C18" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D18" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="E18" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="F18" t="s">
+        <v>191</v>
+      </c>
+      <c r="G18" t="s">
+        <v>190</v>
+      </c>
+      <c r="H18" t="s">
+        <v>187</v>
+      </c>
+      <c r="I18" t="s">
         <v>199</v>
-      </c>
-      <c r="G18" t="s">
-        <v>198</v>
-      </c>
-      <c r="H18" t="s">
-        <v>195</v>
-      </c>
-      <c r="I18" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
@@ -1657,31 +1644,31 @@
     </row>
     <row r="21" spans="1:9" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>136</v>
+        <v>203</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>136</v>
+        <v>202</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>137</v>
+        <v>204</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>138</v>
+        <v>205</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>139</v>
+        <v>206</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>140</v>
+        <v>207</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>141</v>
+        <v>208</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>142</v>
+        <v>210</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>178</v>
+        <v>209</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
@@ -1710,7 +1697,7 @@
         <v>88</v>
       </c>
       <c r="I22" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
@@ -1718,86 +1705,86 @@
         <v>43</v>
       </c>
       <c r="B23" t="s">
+        <v>153</v>
+      </c>
+      <c r="C23" t="s">
+        <v>158</v>
+      </c>
+      <c r="D23" t="s">
         <v>160</v>
       </c>
-      <c r="C23" t="s">
-        <v>165</v>
-      </c>
-      <c r="D23" t="s">
-        <v>167</v>
-      </c>
       <c r="E23" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="F23" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="G23" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="H23" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="I23" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="B24" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="C24" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="D24" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="E24" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="F24" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="G24" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="H24" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="I24" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
@@ -1808,25 +1795,25 @@
         <v>44</v>
       </c>
       <c r="C26" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="D26" t="s">
         <v>73</v>
       </c>
       <c r="E26" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="F26" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="G26" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="H26" t="s">
         <v>133</v>
       </c>
       <c r="I26" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
@@ -1855,7 +1842,7 @@
         <v>134</v>
       </c>
       <c r="I27" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>